<commit_message>
Reading pdf part added The driver script extended for the select flight page as well and can be easily extended for other pages Corresponding test data and properties file updated Changes made to click Action method in class SeleniumActionFunctions so that now the click is made using the javascript executor efficient waiting for the page to load method also added
</commit_message>
<xml_diff>
--- a/resources/input/Data.xlsx
+++ b/resources/input/Data.xlsx
@@ -257,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
   <si>
     <t>TestCase</t>
   </si>
@@ -372,9 +372,6 @@
     <t>NeedFlight</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>automation@bcstechnology.com.au</t>
   </si>
   <si>
@@ -384,18 +381,12 @@
     <t>test1</t>
   </si>
   <si>
-    <t>Starter Plus</t>
-  </si>
-  <si>
     <t>TC_003</t>
   </si>
   <si>
     <t>test2</t>
   </si>
   <si>
-    <t>Starter Max</t>
-  </si>
-  <si>
     <t>TC_004</t>
   </si>
   <si>
@@ -405,12 +396,6 @@
     <t>test4</t>
   </si>
   <si>
-    <t>CheapFlight</t>
-  </si>
-  <si>
-    <t>Business Max</t>
-  </si>
-  <si>
     <t>TC_006</t>
   </si>
   <si>
@@ -463,6 +448,27 @@
   </si>
   <si>
     <t>ADL</t>
+  </si>
+  <si>
+    <t>Plus</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>FlightChoice</t>
+  </si>
+  <si>
+    <t>FlightChoice1</t>
+  </si>
+  <si>
+    <t>FlightChoice4</t>
+  </si>
+  <si>
+    <t>FlightChoice7</t>
+  </si>
+  <si>
+    <t>FlightChoice10</t>
   </si>
 </sst>
 </file>
@@ -888,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,23 +913,22 @@
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1"/>
-    <col min="20" max="20" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" customWidth="1"/>
-    <col min="23" max="23" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" customWidth="1"/>
+    <col min="21" max="21" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -958,72 +963,75 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G2" s="5">
         <v>42686</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I2" s="2">
         <v>2</v>
@@ -1038,29 +1046,32 @@
         <v>27</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="3"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
@@ -1069,10 +1080,10 @@
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G3" s="5">
         <v>42580</v>
@@ -1093,9 +1104,11 @@
         <v>27</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -1107,13 +1120,14 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>25</v>
@@ -1122,16 +1136,16 @@
         <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G4" s="5">
         <v>42675</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2">
         <v>2</v>
@@ -1146,9 +1160,11 @@
         <v>27</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1160,13 +1176,14 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>25</v>
@@ -1175,16 +1192,16 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G5" s="5">
         <v>42675</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I5" s="2">
         <v>2</v>
@@ -1199,9 +1216,11 @@
         <v>27</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1213,13 +1232,14 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>25</v>
@@ -1228,10 +1248,10 @@
         <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G6" s="5">
         <v>42680</v>
@@ -1249,12 +1269,14 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -1266,31 +1288,32 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G7" s="5">
         <v>42685</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I7" s="2">
         <v>2</v>
@@ -1302,12 +1325,14 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -1319,31 +1344,32 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I8" s="2">
         <v>5</v>
@@ -1358,9 +1384,11 @@
         <v>27</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1372,31 +1400,32 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -1408,12 +1437,14 @@
         <v>1</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1425,13 +1456,14 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
@@ -1440,10 +1472,10 @@
         <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G10" s="5">
         <v>42721</v>
@@ -1464,9 +1496,11 @@
         <v>27</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -1478,31 +1512,32 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1514,12 +1549,14 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1531,24 +1568,25 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V15:V1048576 U14 V2:V13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W15:W1048576 V14 W2:W13">
       <formula1>"Cash,Credit Card,Agency,Voucher"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M15:M1048576 L14 M2:M13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L14:N14">
       <formula1>"Starter,Starter Plus,Starter Max,Business,Business Max"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15:D1048576 C14 D2:D13">
       <formula1>"RoundTrip,OneWay"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:N11">
       <formula1>FlightChoice</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1"/>
+    <hyperlink ref="U2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>